<commit_message>
Improve spreadsheet and bg images
</commit_message>
<xml_diff>
--- a/Script Generator.xlsx
+++ b/Script Generator.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Shawna\Documents\GitHub\mysterious-messenger\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Shawna\Documents\Github\mysterious-messenger\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9629A0A3-9635-4047-B84C-62F0B0B27C2F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A67C752-5E3F-4E23-8407-FBB15A4A52D4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="12420" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="16440" windowHeight="28440" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Chatroom Instructions" sheetId="9" r:id="rId1"/>
@@ -2611,7 +2611,7 @@
       <pane xSplit="14" ySplit="1" topLeftCell="O2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="O1" sqref="O1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2723,7 +2723,7 @@
       <c r="J2" s="40"/>
       <c r="K2" s="33"/>
       <c r="L2" s="40" t="str">
-        <f>IF(OR(ISNUMBER(SEARCH("{image",B2)), ISNUMBER(SEARCH(".png", B2)), ISNUMBER(SEARCH(".jpg", B2))),"x","")</f>
+        <f>IF(OR(ISNUMBER(SEARCH("{image",LOWER(B2))), ISNUMBER(SEARCH(".png", LOWER(B2))), ISNUMBER(SEARCH(".jpg", LOWER(B2))), ISNUMBER(SEARCH(".webp", LOWER(B2)))),"x","")</f>
         <v/>
       </c>
       <c r="M2" s="24" t="str">
@@ -2797,7 +2797,7 @@
       <c r="J3" s="40"/>
       <c r="K3" s="33"/>
       <c r="L3" s="40" t="str">
-        <f>IF(OR(ISNUMBER(SEARCH("{image",B3)), ISNUMBER(SEARCH(".png", B3)), ISNUMBER(SEARCH(".jpg", B3))),"x","")</f>
+        <f t="shared" ref="L3:L66" si="3">IF(OR(ISNUMBER(SEARCH("{image",LOWER(B3))), ISNUMBER(SEARCH(".png", LOWER(B3))), ISNUMBER(SEARCH(".jpg", LOWER(B3))), ISNUMBER(SEARCH(".webp", LOWER(B3)))),"x","")</f>
         <v/>
       </c>
       <c r="M3" s="24" t="str">
@@ -2806,11 +2806,11 @@
       </c>
       <c r="N3" s="40"/>
       <c r="P3" t="str">
-        <f t="shared" ref="P3:P66" si="3">IF(B3="","",CONCATENATE(Q3," """,R3,IF(K3&lt;&gt;"","{size=+10}",""),B3,IF(K3&lt;&gt;"","{/size}",""),S3,"""",IF(X3&lt;&gt;"",CONCATENATE(" ",X3),"")))</f>
+        <f t="shared" ref="P3:P66" si="4">IF(B3="","",CONCATENATE(Q3," """,R3,IF(K3&lt;&gt;"","{size=+10}",""),B3,IF(K3&lt;&gt;"","{/size}",""),S3,"""",IF(X3&lt;&gt;"",CONCATENATE(" ",X3),"")))</f>
         <v/>
       </c>
       <c r="Q3" s="1" t="str">
-        <f t="shared" ref="Q3:Q66" si="4">IF(OR(LOWER(A3)="seven", LOWER(A3)="s", LOWER(A3)="707"),"s",
+        <f t="shared" ref="Q3:Q66" si="5">IF(OR(LOWER(A3)="seven", LOWER(A3)="s", LOWER(A3)="707"),"s",
     IF(OR(LOWER(A3)="yoosung", LOWER(A3)="y"),"y",
     IF(OR(LOWER(A3)="mc", LOWER(A3)="m"),"m",
     IF(OR(LOWER(A3)="jumin", LOWER(A3)="ju"),"ju",
@@ -2824,7 +2824,7 @@
         <v>Unknown Character</v>
       </c>
       <c r="R3" t="str">
-        <f t="shared" ref="R3:R66" si="5">IF(D3&lt;&gt;"",CONCATENATE("{=sser1",J3,"}"),IF(E3&lt;&gt;"",CONCATENATE("{=sser2",J3,"}"),IF(F3&lt;&gt;"",CONCATENATE("{=ser1",J3,"}"),IF(G3&lt;&gt;"",CONCATENATE("{=ser2",J3,"}"),IF(H3&lt;&gt;"","{=curly}",IF(I3&lt;&gt;"","{=blocky}",""))))))</f>
+        <f t="shared" ref="R3:R66" si="6">IF(D3&lt;&gt;"",CONCATENATE("{=sser1",J3,"}"),IF(E3&lt;&gt;"",CONCATENATE("{=sser2",J3,"}"),IF(F3&lt;&gt;"",CONCATENATE("{=ser1",J3,"}"),IF(G3&lt;&gt;"",CONCATENATE("{=ser2",J3,"}"),IF(H3&lt;&gt;"","{=curly}",IF(I3&lt;&gt;"","{=blocky}",""))))))</f>
         <v/>
       </c>
       <c r="S3" t="str">
@@ -2832,19 +2832,19 @@
         <v/>
       </c>
       <c r="T3" t="str">
-        <f t="shared" ref="T3:T66" si="6">IF(C3&lt;&gt;"",CONCATENATE("pauseVal=",C3),"")</f>
+        <f t="shared" ref="T3:T66" si="7">IF(C3&lt;&gt;"",CONCATENATE("pauseVal=",C3),"")</f>
         <v/>
       </c>
       <c r="U3" t="str">
-        <f t="shared" ref="U3:U66" si="7">IF(L3&lt;&gt;"","img=True","")</f>
+        <f t="shared" ref="U3:U66" si="8">IF(L3&lt;&gt;"","img=True","")</f>
         <v/>
       </c>
       <c r="V3" t="str">
-        <f t="shared" ref="V3:V66" si="8">IF(M3&lt;&gt;"","bounce=True","")</f>
+        <f t="shared" ref="V3:V66" si="9">IF(M3&lt;&gt;"","bounce=True","")</f>
         <v/>
       </c>
       <c r="W3" t="str">
-        <f t="shared" ref="W3:W66" si="9">IF(N3&lt;&gt;"",CONCATENATE("specBubble=""",N3,""""),"")</f>
+        <f t="shared" ref="W3:W66" si="10">IF(N3&lt;&gt;"",CONCATENATE("specBubble=""",N3,""""),"")</f>
         <v/>
       </c>
       <c r="X3" t="str">
@@ -2860,7 +2860,7 @@
         <v/>
       </c>
       <c r="D4" s="40" t="str">
-        <f t="shared" ref="D3:D66" si="10">IF(AND(OR(J4="b",J4="xb"),E4="", F4="", G4=""),"x","")</f>
+        <f t="shared" ref="D4:D66" si="11">IF(AND(OR(J4="b",J4="xb"),E4="", F4="", G4=""),"x","")</f>
         <v/>
       </c>
       <c r="E4" s="32"/>
@@ -2871,24 +2871,24 @@
       <c r="J4" s="41"/>
       <c r="K4" s="32"/>
       <c r="L4" s="40" t="str">
-        <f t="shared" ref="L3:L66" si="11">IF(OR(ISNUMBER(SEARCH("{image",B4)), ISNUMBER(SEARCH(".png", B4)), ISNUMBER(SEARCH(".jpg", B4))),"x","")</f>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="M4" s="24" t="str">
-        <f t="shared" ref="M3:M66" si="12">IF(N4&lt;&gt;"","x","")</f>
+        <f t="shared" ref="M4:M66" si="12">IF(N4&lt;&gt;"","x","")</f>
         <v/>
       </c>
       <c r="N4" s="41"/>
       <c r="P4" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="Q4" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>Unknown Character</v>
       </c>
       <c r="R4" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="S4" t="str">
@@ -2896,19 +2896,19 @@
         <v/>
       </c>
       <c r="T4" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="U4" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="V4" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="W4" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="X4" t="str">
@@ -2924,7 +2924,7 @@
         <v/>
       </c>
       <c r="D5" s="40" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v/>
       </c>
       <c r="E5" s="32"/>
@@ -2935,7 +2935,7 @@
       <c r="J5" s="41"/>
       <c r="K5" s="32"/>
       <c r="L5" s="40" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="M5" s="24" t="str">
@@ -2944,15 +2944,15 @@
       </c>
       <c r="N5" s="41"/>
       <c r="P5" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="Q5" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>Unknown Character</v>
       </c>
       <c r="R5" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="S5" t="str">
@@ -2960,19 +2960,19 @@
         <v/>
       </c>
       <c r="T5" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="U5" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="V5" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="W5" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="X5" t="str">
@@ -2988,7 +2988,7 @@
         <v/>
       </c>
       <c r="D6" s="40" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v/>
       </c>
       <c r="E6" s="32"/>
@@ -2999,7 +2999,7 @@
       <c r="J6" s="41"/>
       <c r="K6" s="32"/>
       <c r="L6" s="40" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="M6" s="24" t="str">
@@ -3008,15 +3008,15 @@
       </c>
       <c r="N6" s="41"/>
       <c r="P6" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="Q6" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>Unknown Character</v>
       </c>
       <c r="R6" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="S6" t="str">
@@ -3024,19 +3024,19 @@
         <v/>
       </c>
       <c r="T6" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="U6" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="V6" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="W6" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="X6" t="str">
@@ -3052,7 +3052,7 @@
         <v/>
       </c>
       <c r="D7" s="40" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v/>
       </c>
       <c r="E7" s="32"/>
@@ -3063,7 +3063,7 @@
       <c r="J7" s="41"/>
       <c r="K7" s="32"/>
       <c r="L7" s="40" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="M7" s="24" t="str">
@@ -3072,15 +3072,15 @@
       </c>
       <c r="N7" s="41"/>
       <c r="P7" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="Q7" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>Unknown Character</v>
       </c>
       <c r="R7" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="S7" t="str">
@@ -3088,19 +3088,19 @@
         <v/>
       </c>
       <c r="T7" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="U7" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="V7" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="W7" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="X7" t="str">
@@ -3116,7 +3116,7 @@
         <v/>
       </c>
       <c r="D8" s="40" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v/>
       </c>
       <c r="E8" s="32"/>
@@ -3127,7 +3127,7 @@
       <c r="J8" s="41"/>
       <c r="K8" s="32"/>
       <c r="L8" s="40" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="M8" s="24" t="str">
@@ -3136,15 +3136,15 @@
       </c>
       <c r="N8" s="41"/>
       <c r="P8" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="Q8" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>Unknown Character</v>
       </c>
       <c r="R8" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="S8" t="str">
@@ -3152,19 +3152,19 @@
         <v/>
       </c>
       <c r="T8" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="U8" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="V8" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="W8" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="X8" t="str">
@@ -3180,7 +3180,7 @@
         <v/>
       </c>
       <c r="D9" s="40" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v/>
       </c>
       <c r="E9" s="32"/>
@@ -3191,7 +3191,7 @@
       <c r="J9" s="41"/>
       <c r="K9" s="32"/>
       <c r="L9" s="40" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="M9" s="24" t="str">
@@ -3200,15 +3200,15 @@
       </c>
       <c r="N9" s="41"/>
       <c r="P9" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="Q9" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>Unknown Character</v>
       </c>
       <c r="R9" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="S9" t="str">
@@ -3216,19 +3216,19 @@
         <v/>
       </c>
       <c r="T9" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="U9" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="V9" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="W9" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="X9" t="str">
@@ -3244,7 +3244,7 @@
         <v/>
       </c>
       <c r="D10" s="40" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v/>
       </c>
       <c r="E10" s="32"/>
@@ -3255,7 +3255,7 @@
       <c r="J10" s="41"/>
       <c r="K10" s="32"/>
       <c r="L10" s="40" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="M10" s="24" t="str">
@@ -3264,15 +3264,15 @@
       </c>
       <c r="N10" s="41"/>
       <c r="P10" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="Q10" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>Unknown Character</v>
       </c>
       <c r="R10" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="S10" t="str">
@@ -3280,19 +3280,19 @@
         <v/>
       </c>
       <c r="T10" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="U10" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="V10" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="W10" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="X10" t="str">
@@ -3307,11 +3307,11 @@
         <v/>
       </c>
       <c r="D11" s="40" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v/>
       </c>
       <c r="L11" s="40" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="M11" s="24" t="str">
@@ -3319,15 +3319,15 @@
         <v/>
       </c>
       <c r="P11" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="Q11" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>Unknown Character</v>
       </c>
       <c r="R11" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="S11" t="str">
@@ -3335,19 +3335,19 @@
         <v/>
       </c>
       <c r="T11" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="U11" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="V11" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="W11" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="X11" t="str">
@@ -3362,11 +3362,11 @@
         <v/>
       </c>
       <c r="D12" s="40" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v/>
       </c>
       <c r="L12" s="40" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="M12" s="24" t="str">
@@ -3374,15 +3374,15 @@
         <v/>
       </c>
       <c r="P12" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="Q12" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>Unknown Character</v>
       </c>
       <c r="R12" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="S12" t="str">
@@ -3390,19 +3390,19 @@
         <v/>
       </c>
       <c r="T12" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="U12" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="V12" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="W12" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="X12" t="str">
@@ -3416,11 +3416,11 @@
         <v/>
       </c>
       <c r="D13" s="40" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v/>
       </c>
       <c r="L13" s="40" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="M13" s="24" t="str">
@@ -3428,15 +3428,15 @@
         <v/>
       </c>
       <c r="P13" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="Q13" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>Unknown Character</v>
       </c>
       <c r="R13" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="S13" t="str">
@@ -3444,19 +3444,19 @@
         <v/>
       </c>
       <c r="T13" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="U13" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="V13" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="W13" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="X13" t="str">
@@ -3470,11 +3470,11 @@
         <v/>
       </c>
       <c r="D14" s="40" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v/>
       </c>
       <c r="L14" s="40" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="M14" s="24" t="str">
@@ -3482,15 +3482,15 @@
         <v/>
       </c>
       <c r="P14" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="Q14" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>Unknown Character</v>
       </c>
       <c r="R14" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="S14" t="str">
@@ -3498,19 +3498,19 @@
         <v/>
       </c>
       <c r="T14" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="U14" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="V14" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="W14" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="X14" t="str">
@@ -3524,11 +3524,11 @@
         <v/>
       </c>
       <c r="D15" s="40" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v/>
       </c>
       <c r="L15" s="40" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="M15" s="24" t="str">
@@ -3536,15 +3536,15 @@
         <v/>
       </c>
       <c r="P15" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="Q15" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>Unknown Character</v>
       </c>
       <c r="R15" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="S15" t="str">
@@ -3552,19 +3552,19 @@
         <v/>
       </c>
       <c r="T15" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="U15" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="V15" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="W15" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="X15" t="str">
@@ -3578,11 +3578,11 @@
         <v/>
       </c>
       <c r="D16" s="40" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v/>
       </c>
       <c r="L16" s="40" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="M16" s="24" t="str">
@@ -3590,15 +3590,15 @@
         <v/>
       </c>
       <c r="P16" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="Q16" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>Unknown Character</v>
       </c>
       <c r="R16" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="S16" t="str">
@@ -3606,19 +3606,19 @@
         <v/>
       </c>
       <c r="T16" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="U16" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="V16" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="W16" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="X16" t="str">
@@ -3632,11 +3632,11 @@
         <v/>
       </c>
       <c r="D17" s="40" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v/>
       </c>
       <c r="L17" s="40" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="M17" s="24" t="str">
@@ -3644,15 +3644,15 @@
         <v/>
       </c>
       <c r="P17" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="Q17" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>Unknown Character</v>
       </c>
       <c r="R17" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="S17" t="str">
@@ -3660,19 +3660,19 @@
         <v/>
       </c>
       <c r="T17" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="U17" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="V17" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="W17" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="X17" t="str">
@@ -3686,11 +3686,11 @@
         <v/>
       </c>
       <c r="D18" s="40" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v/>
       </c>
       <c r="L18" s="40" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="M18" s="24" t="str">
@@ -3698,15 +3698,15 @@
         <v/>
       </c>
       <c r="P18" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="Q18" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>Unknown Character</v>
       </c>
       <c r="R18" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="S18" t="str">
@@ -3714,19 +3714,19 @@
         <v/>
       </c>
       <c r="T18" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="U18" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="V18" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="W18" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="X18" t="str">
@@ -3740,11 +3740,11 @@
         <v/>
       </c>
       <c r="D19" s="40" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v/>
       </c>
       <c r="L19" s="40" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="M19" s="24" t="str">
@@ -3752,15 +3752,15 @@
         <v/>
       </c>
       <c r="P19" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="Q19" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>Unknown Character</v>
       </c>
       <c r="R19" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="S19" t="str">
@@ -3768,19 +3768,19 @@
         <v/>
       </c>
       <c r="T19" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="U19" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="V19" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="W19" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="X19" t="str">
@@ -3794,11 +3794,11 @@
         <v/>
       </c>
       <c r="D20" s="40" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v/>
       </c>
       <c r="L20" s="40" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="M20" s="24" t="str">
@@ -3806,15 +3806,15 @@
         <v/>
       </c>
       <c r="P20" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="Q20" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>Unknown Character</v>
       </c>
       <c r="R20" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="S20" t="str">
@@ -3822,19 +3822,19 @@
         <v/>
       </c>
       <c r="T20" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="U20" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="V20" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="W20" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="X20" t="str">
@@ -3848,11 +3848,11 @@
         <v/>
       </c>
       <c r="D21" s="40" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v/>
       </c>
       <c r="L21" s="40" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="M21" s="24" t="str">
@@ -3860,15 +3860,15 @@
         <v/>
       </c>
       <c r="P21" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="Q21" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>Unknown Character</v>
       </c>
       <c r="R21" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="S21" t="str">
@@ -3876,19 +3876,19 @@
         <v/>
       </c>
       <c r="T21" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="U21" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="V21" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="W21" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="X21" t="str">
@@ -3902,11 +3902,11 @@
         <v/>
       </c>
       <c r="D22" s="40" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v/>
       </c>
       <c r="L22" s="40" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="M22" s="24" t="str">
@@ -3914,15 +3914,15 @@
         <v/>
       </c>
       <c r="P22" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="Q22" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>Unknown Character</v>
       </c>
       <c r="R22" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="S22" t="str">
@@ -3930,19 +3930,19 @@
         <v/>
       </c>
       <c r="T22" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="U22" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="V22" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="W22" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="X22" t="str">
@@ -3956,11 +3956,11 @@
         <v/>
       </c>
       <c r="D23" s="40" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v/>
       </c>
       <c r="L23" s="40" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="M23" s="24" t="str">
@@ -3968,15 +3968,15 @@
         <v/>
       </c>
       <c r="P23" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="Q23" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>Unknown Character</v>
       </c>
       <c r="R23" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="S23" t="str">
@@ -3984,19 +3984,19 @@
         <v/>
       </c>
       <c r="T23" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="U23" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="V23" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="W23" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="X23" t="str">
@@ -4010,11 +4010,11 @@
         <v/>
       </c>
       <c r="D24" s="40" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v/>
       </c>
       <c r="L24" s="40" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="M24" s="24" t="str">
@@ -4022,15 +4022,15 @@
         <v/>
       </c>
       <c r="P24" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="Q24" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>Unknown Character</v>
       </c>
       <c r="R24" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="S24" t="str">
@@ -4038,19 +4038,19 @@
         <v/>
       </c>
       <c r="T24" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="U24" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="V24" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="W24" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="X24" t="str">
@@ -4064,11 +4064,11 @@
         <v/>
       </c>
       <c r="D25" s="40" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v/>
       </c>
       <c r="L25" s="40" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="M25" s="24" t="str">
@@ -4076,15 +4076,15 @@
         <v/>
       </c>
       <c r="P25" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="Q25" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>Unknown Character</v>
       </c>
       <c r="R25" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="S25" t="str">
@@ -4092,19 +4092,19 @@
         <v/>
       </c>
       <c r="T25" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="U25" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="V25" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="W25" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="X25" t="str">
@@ -4118,11 +4118,11 @@
         <v/>
       </c>
       <c r="D26" s="40" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v/>
       </c>
       <c r="L26" s="40" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="M26" s="24" t="str">
@@ -4130,15 +4130,15 @@
         <v/>
       </c>
       <c r="P26" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="Q26" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>Unknown Character</v>
       </c>
       <c r="R26" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="S26" t="str">
@@ -4146,19 +4146,19 @@
         <v/>
       </c>
       <c r="T26" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="U26" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="V26" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="W26" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="X26" t="str">
@@ -4172,11 +4172,11 @@
         <v/>
       </c>
       <c r="D27" s="40" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v/>
       </c>
       <c r="L27" s="40" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="M27" s="24" t="str">
@@ -4184,15 +4184,15 @@
         <v/>
       </c>
       <c r="P27" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="Q27" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>Unknown Character</v>
       </c>
       <c r="R27" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="S27" t="str">
@@ -4200,19 +4200,19 @@
         <v/>
       </c>
       <c r="T27" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="U27" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="V27" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="W27" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="X27" t="str">
@@ -4226,11 +4226,11 @@
         <v/>
       </c>
       <c r="D28" s="40" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v/>
       </c>
       <c r="L28" s="40" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="M28" s="24" t="str">
@@ -4238,15 +4238,15 @@
         <v/>
       </c>
       <c r="P28" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="Q28" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>Unknown Character</v>
       </c>
       <c r="R28" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="S28" t="str">
@@ -4254,19 +4254,19 @@
         <v/>
       </c>
       <c r="T28" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="U28" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="V28" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="W28" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="X28" t="str">
@@ -4280,11 +4280,11 @@
         <v/>
       </c>
       <c r="D29" s="40" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v/>
       </c>
       <c r="L29" s="40" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="M29" s="24" t="str">
@@ -4292,15 +4292,15 @@
         <v/>
       </c>
       <c r="P29" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="Q29" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>Unknown Character</v>
       </c>
       <c r="R29" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="S29" t="str">
@@ -4308,19 +4308,19 @@
         <v/>
       </c>
       <c r="T29" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="U29" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="V29" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="W29" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="X29" t="str">
@@ -4334,11 +4334,11 @@
         <v/>
       </c>
       <c r="D30" s="40" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v/>
       </c>
       <c r="L30" s="40" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="M30" s="24" t="str">
@@ -4346,15 +4346,15 @@
         <v/>
       </c>
       <c r="P30" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="Q30" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>Unknown Character</v>
       </c>
       <c r="R30" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="S30" t="str">
@@ -4362,19 +4362,19 @@
         <v/>
       </c>
       <c r="T30" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="U30" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="V30" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="W30" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="X30" t="str">
@@ -4388,11 +4388,11 @@
         <v/>
       </c>
       <c r="D31" s="40" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v/>
       </c>
       <c r="L31" s="40" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="M31" s="24" t="str">
@@ -4400,15 +4400,15 @@
         <v/>
       </c>
       <c r="P31" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="Q31" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>Unknown Character</v>
       </c>
       <c r="R31" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="S31" t="str">
@@ -4416,19 +4416,19 @@
         <v/>
       </c>
       <c r="T31" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="U31" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="V31" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="W31" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="X31" t="str">
@@ -4442,11 +4442,11 @@
         <v/>
       </c>
       <c r="D32" s="40" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v/>
       </c>
       <c r="L32" s="40" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="M32" s="24" t="str">
@@ -4454,15 +4454,15 @@
         <v/>
       </c>
       <c r="P32" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="Q32" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>Unknown Character</v>
       </c>
       <c r="R32" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="S32" t="str">
@@ -4470,19 +4470,19 @@
         <v/>
       </c>
       <c r="T32" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="U32" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="V32" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="W32" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="X32" t="str">
@@ -4496,11 +4496,11 @@
         <v/>
       </c>
       <c r="D33" s="40" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v/>
       </c>
       <c r="L33" s="40" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="M33" s="24" t="str">
@@ -4508,15 +4508,15 @@
         <v/>
       </c>
       <c r="P33" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="Q33" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>Unknown Character</v>
       </c>
       <c r="R33" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="S33" t="str">
@@ -4524,19 +4524,19 @@
         <v/>
       </c>
       <c r="T33" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="U33" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="V33" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="W33" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="X33" t="str">
@@ -4550,11 +4550,11 @@
         <v/>
       </c>
       <c r="D34" s="40" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v/>
       </c>
       <c r="L34" s="40" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="M34" s="24" t="str">
@@ -4562,15 +4562,15 @@
         <v/>
       </c>
       <c r="P34" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="Q34" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>Unknown Character</v>
       </c>
       <c r="R34" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="S34" t="str">
@@ -4578,19 +4578,19 @@
         <v/>
       </c>
       <c r="T34" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="U34" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="V34" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="W34" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="X34" t="str">
@@ -4604,11 +4604,11 @@
         <v/>
       </c>
       <c r="D35" s="40" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v/>
       </c>
       <c r="L35" s="40" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="M35" s="24" t="str">
@@ -4616,15 +4616,15 @@
         <v/>
       </c>
       <c r="P35" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="Q35" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>Unknown Character</v>
       </c>
       <c r="R35" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="S35" t="str">
@@ -4632,19 +4632,19 @@
         <v/>
       </c>
       <c r="T35" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="U35" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="V35" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="W35" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="X35" t="str">
@@ -4658,11 +4658,11 @@
         <v/>
       </c>
       <c r="D36" s="40" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v/>
       </c>
       <c r="L36" s="40" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="M36" s="24" t="str">
@@ -4670,15 +4670,15 @@
         <v/>
       </c>
       <c r="P36" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="Q36" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>Unknown Character</v>
       </c>
       <c r="R36" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="S36" t="str">
@@ -4686,19 +4686,19 @@
         <v/>
       </c>
       <c r="T36" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="U36" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="V36" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="W36" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="X36" t="str">
@@ -4712,11 +4712,11 @@
         <v/>
       </c>
       <c r="D37" s="40" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v/>
       </c>
       <c r="L37" s="40" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="M37" s="24" t="str">
@@ -4724,15 +4724,15 @@
         <v/>
       </c>
       <c r="P37" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="Q37" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>Unknown Character</v>
       </c>
       <c r="R37" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="S37" t="str">
@@ -4740,19 +4740,19 @@
         <v/>
       </c>
       <c r="T37" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="U37" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="V37" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="W37" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="X37" t="str">
@@ -4766,11 +4766,11 @@
         <v/>
       </c>
       <c r="D38" s="40" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v/>
       </c>
       <c r="L38" s="40" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="M38" s="24" t="str">
@@ -4778,15 +4778,15 @@
         <v/>
       </c>
       <c r="P38" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="Q38" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>Unknown Character</v>
       </c>
       <c r="R38" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="S38" t="str">
@@ -4794,19 +4794,19 @@
         <v/>
       </c>
       <c r="T38" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="U38" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="V38" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="W38" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="X38" t="str">
@@ -4820,11 +4820,11 @@
         <v/>
       </c>
       <c r="D39" s="40" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v/>
       </c>
       <c r="L39" s="40" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="M39" s="24" t="str">
@@ -4832,15 +4832,15 @@
         <v/>
       </c>
       <c r="P39" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="Q39" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>Unknown Character</v>
       </c>
       <c r="R39" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="S39" t="str">
@@ -4848,19 +4848,19 @@
         <v/>
       </c>
       <c r="T39" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="U39" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="V39" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="W39" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="X39" t="str">
@@ -4874,11 +4874,11 @@
         <v/>
       </c>
       <c r="D40" s="40" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v/>
       </c>
       <c r="L40" s="40" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="M40" s="24" t="str">
@@ -4886,15 +4886,15 @@
         <v/>
       </c>
       <c r="P40" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="Q40" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>Unknown Character</v>
       </c>
       <c r="R40" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="S40" t="str">
@@ -4902,19 +4902,19 @@
         <v/>
       </c>
       <c r="T40" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="U40" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="V40" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="W40" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="X40" t="str">
@@ -4928,11 +4928,11 @@
         <v/>
       </c>
       <c r="D41" s="40" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v/>
       </c>
       <c r="L41" s="40" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="M41" s="24" t="str">
@@ -4940,15 +4940,15 @@
         <v/>
       </c>
       <c r="P41" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="Q41" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>Unknown Character</v>
       </c>
       <c r="R41" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="S41" t="str">
@@ -4956,19 +4956,19 @@
         <v/>
       </c>
       <c r="T41" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="U41" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="V41" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="W41" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="X41" t="str">
@@ -4982,11 +4982,11 @@
         <v/>
       </c>
       <c r="D42" s="40" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v/>
       </c>
       <c r="L42" s="40" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="M42" s="24" t="str">
@@ -4994,15 +4994,15 @@
         <v/>
       </c>
       <c r="P42" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="Q42" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>Unknown Character</v>
       </c>
       <c r="R42" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="S42" t="str">
@@ -5010,19 +5010,19 @@
         <v/>
       </c>
       <c r="T42" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="U42" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="V42" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="W42" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="X42" t="str">
@@ -5036,11 +5036,11 @@
         <v/>
       </c>
       <c r="D43" s="40" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v/>
       </c>
       <c r="L43" s="40" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="M43" s="24" t="str">
@@ -5048,15 +5048,15 @@
         <v/>
       </c>
       <c r="P43" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="Q43" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>Unknown Character</v>
       </c>
       <c r="R43" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="S43" t="str">
@@ -5064,19 +5064,19 @@
         <v/>
       </c>
       <c r="T43" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="U43" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="V43" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="W43" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="X43" t="str">
@@ -5090,11 +5090,11 @@
         <v/>
       </c>
       <c r="D44" s="40" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v/>
       </c>
       <c r="L44" s="40" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="M44" s="24" t="str">
@@ -5102,15 +5102,15 @@
         <v/>
       </c>
       <c r="P44" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="Q44" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>Unknown Character</v>
       </c>
       <c r="R44" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="S44" t="str">
@@ -5118,19 +5118,19 @@
         <v/>
       </c>
       <c r="T44" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="U44" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="V44" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="W44" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="X44" t="str">
@@ -5144,11 +5144,11 @@
         <v/>
       </c>
       <c r="D45" s="40" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v/>
       </c>
       <c r="L45" s="40" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="M45" s="24" t="str">
@@ -5156,15 +5156,15 @@
         <v/>
       </c>
       <c r="P45" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="Q45" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>Unknown Character</v>
       </c>
       <c r="R45" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="S45" t="str">
@@ -5172,19 +5172,19 @@
         <v/>
       </c>
       <c r="T45" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="U45" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="V45" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="W45" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="X45" t="str">
@@ -5198,11 +5198,11 @@
         <v/>
       </c>
       <c r="D46" s="40" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v/>
       </c>
       <c r="L46" s="40" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="M46" s="24" t="str">
@@ -5210,15 +5210,15 @@
         <v/>
       </c>
       <c r="P46" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="Q46" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>Unknown Character</v>
       </c>
       <c r="R46" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="S46" t="str">
@@ -5226,19 +5226,19 @@
         <v/>
       </c>
       <c r="T46" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="U46" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="V46" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="W46" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="X46" t="str">
@@ -5252,11 +5252,11 @@
         <v/>
       </c>
       <c r="D47" s="40" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v/>
       </c>
       <c r="L47" s="40" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="M47" s="24" t="str">
@@ -5264,15 +5264,15 @@
         <v/>
       </c>
       <c r="P47" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="Q47" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>Unknown Character</v>
       </c>
       <c r="R47" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="S47" t="str">
@@ -5280,19 +5280,19 @@
         <v/>
       </c>
       <c r="T47" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="U47" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="V47" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="W47" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="X47" t="str">
@@ -5306,11 +5306,11 @@
         <v/>
       </c>
       <c r="D48" s="40" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v/>
       </c>
       <c r="L48" s="40" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="M48" s="24" t="str">
@@ -5318,15 +5318,15 @@
         <v/>
       </c>
       <c r="P48" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="Q48" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>Unknown Character</v>
       </c>
       <c r="R48" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="S48" t="str">
@@ -5334,19 +5334,19 @@
         <v/>
       </c>
       <c r="T48" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="U48" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="V48" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="W48" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="X48" t="str">
@@ -5360,11 +5360,11 @@
         <v/>
       </c>
       <c r="D49" s="40" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v/>
       </c>
       <c r="L49" s="40" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="M49" s="24" t="str">
@@ -5372,15 +5372,15 @@
         <v/>
       </c>
       <c r="P49" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="Q49" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>Unknown Character</v>
       </c>
       <c r="R49" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="S49" t="str">
@@ -5388,19 +5388,19 @@
         <v/>
       </c>
       <c r="T49" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="U49" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="V49" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="W49" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="X49" t="str">
@@ -5414,11 +5414,11 @@
         <v/>
       </c>
       <c r="D50" s="40" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v/>
       </c>
       <c r="L50" s="40" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="M50" s="24" t="str">
@@ -5426,15 +5426,15 @@
         <v/>
       </c>
       <c r="P50" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="Q50" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>Unknown Character</v>
       </c>
       <c r="R50" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="S50" t="str">
@@ -5442,19 +5442,19 @@
         <v/>
       </c>
       <c r="T50" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="U50" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="V50" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="W50" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="X50" t="str">
@@ -5468,11 +5468,11 @@
         <v/>
       </c>
       <c r="D51" s="40" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v/>
       </c>
       <c r="L51" s="40" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="M51" s="24" t="str">
@@ -5480,15 +5480,15 @@
         <v/>
       </c>
       <c r="P51" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="Q51" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>Unknown Character</v>
       </c>
       <c r="R51" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="S51" t="str">
@@ -5496,19 +5496,19 @@
         <v/>
       </c>
       <c r="T51" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="U51" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="V51" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="W51" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="X51" t="str">
@@ -5522,11 +5522,11 @@
         <v/>
       </c>
       <c r="D52" s="40" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v/>
       </c>
       <c r="L52" s="40" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="M52" s="24" t="str">
@@ -5534,15 +5534,15 @@
         <v/>
       </c>
       <c r="P52" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="Q52" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>Unknown Character</v>
       </c>
       <c r="R52" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="S52" t="str">
@@ -5550,19 +5550,19 @@
         <v/>
       </c>
       <c r="T52" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="U52" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="V52" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="W52" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="X52" t="str">
@@ -5576,11 +5576,11 @@
         <v/>
       </c>
       <c r="D53" s="40" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v/>
       </c>
       <c r="L53" s="40" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="M53" s="24" t="str">
@@ -5588,15 +5588,15 @@
         <v/>
       </c>
       <c r="P53" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="Q53" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>Unknown Character</v>
       </c>
       <c r="R53" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="S53" t="str">
@@ -5604,19 +5604,19 @@
         <v/>
       </c>
       <c r="T53" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="U53" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="V53" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="W53" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="X53" t="str">
@@ -5630,11 +5630,11 @@
         <v/>
       </c>
       <c r="D54" s="40" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v/>
       </c>
       <c r="L54" s="40" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="M54" s="24" t="str">
@@ -5642,15 +5642,15 @@
         <v/>
       </c>
       <c r="P54" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="Q54" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>Unknown Character</v>
       </c>
       <c r="R54" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="S54" t="str">
@@ -5658,19 +5658,19 @@
         <v/>
       </c>
       <c r="T54" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="U54" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="V54" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="W54" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="X54" t="str">
@@ -5684,11 +5684,11 @@
         <v/>
       </c>
       <c r="D55" s="40" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v/>
       </c>
       <c r="L55" s="40" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="M55" s="24" t="str">
@@ -5696,15 +5696,15 @@
         <v/>
       </c>
       <c r="P55" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="Q55" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>Unknown Character</v>
       </c>
       <c r="R55" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="S55" t="str">
@@ -5712,19 +5712,19 @@
         <v/>
       </c>
       <c r="T55" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="U55" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="V55" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="W55" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="X55" t="str">
@@ -5738,11 +5738,11 @@
         <v/>
       </c>
       <c r="D56" s="40" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v/>
       </c>
       <c r="L56" s="40" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="M56" s="24" t="str">
@@ -5750,15 +5750,15 @@
         <v/>
       </c>
       <c r="P56" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="Q56" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>Unknown Character</v>
       </c>
       <c r="R56" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="S56" t="str">
@@ -5766,19 +5766,19 @@
         <v/>
       </c>
       <c r="T56" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="U56" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="V56" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="W56" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="X56" t="str">
@@ -5792,11 +5792,11 @@
         <v/>
       </c>
       <c r="D57" s="40" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v/>
       </c>
       <c r="L57" s="40" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="M57" s="24" t="str">
@@ -5804,15 +5804,15 @@
         <v/>
       </c>
       <c r="P57" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="Q57" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>Unknown Character</v>
       </c>
       <c r="R57" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="S57" t="str">
@@ -5820,19 +5820,19 @@
         <v/>
       </c>
       <c r="T57" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="U57" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="V57" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="W57" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="X57" t="str">
@@ -5846,11 +5846,11 @@
         <v/>
       </c>
       <c r="D58" s="40" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v/>
       </c>
       <c r="L58" s="40" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="M58" s="24" t="str">
@@ -5858,15 +5858,15 @@
         <v/>
       </c>
       <c r="P58" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="Q58" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>Unknown Character</v>
       </c>
       <c r="R58" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="S58" t="str">
@@ -5874,19 +5874,19 @@
         <v/>
       </c>
       <c r="T58" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="U58" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="V58" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="W58" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="X58" t="str">
@@ -5900,11 +5900,11 @@
         <v/>
       </c>
       <c r="D59" s="40" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v/>
       </c>
       <c r="L59" s="40" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="M59" s="24" t="str">
@@ -5912,15 +5912,15 @@
         <v/>
       </c>
       <c r="P59" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="Q59" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>Unknown Character</v>
       </c>
       <c r="R59" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="S59" t="str">
@@ -5928,19 +5928,19 @@
         <v/>
       </c>
       <c r="T59" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="U59" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="V59" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="W59" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="X59" t="str">
@@ -5954,11 +5954,11 @@
         <v/>
       </c>
       <c r="D60" s="40" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v/>
       </c>
       <c r="L60" s="40" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="M60" s="24" t="str">
@@ -5966,15 +5966,15 @@
         <v/>
       </c>
       <c r="P60" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="Q60" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>Unknown Character</v>
       </c>
       <c r="R60" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="S60" t="str">
@@ -5982,19 +5982,19 @@
         <v/>
       </c>
       <c r="T60" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="U60" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="V60" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="W60" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="X60" t="str">
@@ -6008,11 +6008,11 @@
         <v/>
       </c>
       <c r="D61" s="40" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v/>
       </c>
       <c r="L61" s="40" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="M61" s="24" t="str">
@@ -6020,15 +6020,15 @@
         <v/>
       </c>
       <c r="P61" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="Q61" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>Unknown Character</v>
       </c>
       <c r="R61" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="S61" t="str">
@@ -6036,19 +6036,19 @@
         <v/>
       </c>
       <c r="T61" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="U61" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="V61" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="W61" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="X61" t="str">
@@ -6062,11 +6062,11 @@
         <v/>
       </c>
       <c r="D62" s="40" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v/>
       </c>
       <c r="L62" s="40" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="M62" s="24" t="str">
@@ -6074,15 +6074,15 @@
         <v/>
       </c>
       <c r="P62" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="Q62" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>Unknown Character</v>
       </c>
       <c r="R62" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="S62" t="str">
@@ -6090,19 +6090,19 @@
         <v/>
       </c>
       <c r="T62" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="U62" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="V62" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="W62" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="X62" t="str">
@@ -6116,11 +6116,11 @@
         <v/>
       </c>
       <c r="D63" s="40" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v/>
       </c>
       <c r="L63" s="40" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="M63" s="24" t="str">
@@ -6128,15 +6128,15 @@
         <v/>
       </c>
       <c r="P63" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="Q63" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>Unknown Character</v>
       </c>
       <c r="R63" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="S63" t="str">
@@ -6144,19 +6144,19 @@
         <v/>
       </c>
       <c r="T63" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="U63" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="V63" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="W63" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="X63" t="str">
@@ -6170,11 +6170,11 @@
         <v/>
       </c>
       <c r="D64" s="40" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v/>
       </c>
       <c r="L64" s="40" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="M64" s="24" t="str">
@@ -6182,15 +6182,15 @@
         <v/>
       </c>
       <c r="P64" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="Q64" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>Unknown Character</v>
       </c>
       <c r="R64" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="S64" t="str">
@@ -6198,19 +6198,19 @@
         <v/>
       </c>
       <c r="T64" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="U64" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="V64" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="W64" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="X64" t="str">
@@ -6224,11 +6224,11 @@
         <v/>
       </c>
       <c r="D65" s="40" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v/>
       </c>
       <c r="L65" s="40" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="M65" s="24" t="str">
@@ -6236,15 +6236,15 @@
         <v/>
       </c>
       <c r="P65" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="Q65" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>Unknown Character</v>
       </c>
       <c r="R65" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="S65" t="str">
@@ -6252,19 +6252,19 @@
         <v/>
       </c>
       <c r="T65" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="U65" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="V65" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="W65" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="X65" t="str">
@@ -6278,11 +6278,11 @@
         <v/>
       </c>
       <c r="D66" s="40" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v/>
       </c>
       <c r="L66" s="40" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="M66" s="24" t="str">
@@ -6290,15 +6290,15 @@
         <v/>
       </c>
       <c r="P66" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="Q66" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>Unknown Character</v>
       </c>
       <c r="R66" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="S66" t="str">
@@ -6306,19 +6306,19 @@
         <v/>
       </c>
       <c r="T66" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="U66" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="V66" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="W66" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="X66" t="str">
@@ -6336,7 +6336,7 @@
         <v/>
       </c>
       <c r="L67" s="40" t="str">
-        <f t="shared" ref="L67:L130" si="17">IF(OR(ISNUMBER(SEARCH("{image",B67)), ISNUMBER(SEARCH(".png", B67)), ISNUMBER(SEARCH(".jpg", B67))),"x","")</f>
+        <f t="shared" ref="L67:L130" si="17">IF(OR(ISNUMBER(SEARCH("{image",LOWER(B67))), ISNUMBER(SEARCH(".png", LOWER(B67))), ISNUMBER(SEARCH(".jpg", LOWER(B67))), ISNUMBER(SEARCH(".webp", LOWER(B67)))),"x","")</f>
         <v/>
       </c>
       <c r="M67" s="24" t="str">
@@ -9802,7 +9802,7 @@
         <v/>
       </c>
       <c r="L131" s="40" t="str">
-        <f t="shared" ref="L131:L194" si="30">IF(OR(ISNUMBER(SEARCH("{image",B131)), ISNUMBER(SEARCH(".png", B131)), ISNUMBER(SEARCH(".jpg", B131))),"x","")</f>
+        <f t="shared" ref="L131:L194" si="30">IF(OR(ISNUMBER(SEARCH("{image",LOWER(B131))), ISNUMBER(SEARCH(".png", LOWER(B131))), ISNUMBER(SEARCH(".jpg", LOWER(B131))), ISNUMBER(SEARCH(".webp", LOWER(B131)))),"x","")</f>
         <v/>
       </c>
       <c r="M131" s="24" t="str">
@@ -13268,7 +13268,7 @@
         <v/>
       </c>
       <c r="L195" s="40" t="str">
-        <f t="shared" ref="L195:L251" si="43">IF(OR(ISNUMBER(SEARCH("{image",B195)), ISNUMBER(SEARCH(".png", B195)), ISNUMBER(SEARCH(".jpg", B195))),"x","")</f>
+        <f t="shared" ref="L195:L251" si="43">IF(OR(ISNUMBER(SEARCH("{image",LOWER(B195))), ISNUMBER(SEARCH(".png", LOWER(B195))), ISNUMBER(SEARCH(".jpg", LOWER(B195))), ISNUMBER(SEARCH(".webp", LOWER(B195)))),"x","")</f>
         <v/>
       </c>
       <c r="M195" s="24" t="str">

</xml_diff>

<commit_message>
Trim extra spaces from dialogue
</commit_message>
<xml_diff>
--- a/Script Generator.xlsx
+++ b/Script Generator.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Shawna\Documents\Github\mysterious-messenger\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Shawna\Documents\GitHub\mysterious-messenger\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A67C752-5E3F-4E23-8407-FBB15A4A52D4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAE50471-1E22-4E73-AAE4-0A424E6A79BD}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="16440" windowHeight="28440" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Chatroom Instructions" sheetId="9" r:id="rId1"/>
@@ -2608,10 +2608,10 @@
   <dimension ref="A1:X251"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="14" ySplit="1" topLeftCell="O2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="14" ySplit="1" topLeftCell="O31" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="O1" sqref="O1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="L2" sqref="L2"/>
+      <selection pane="bottomRight" activeCell="P2" sqref="P2:P251"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2732,7 +2732,7 @@
       </c>
       <c r="N2" s="40"/>
       <c r="P2" t="str">
-        <f>IF(B2="","",CONCATENATE(Q2," """,R2,IF(K2&lt;&gt;"","{size=+10}",""),B2,IF(K2&lt;&gt;"","{/size}",""),S2,"""",IF(X2&lt;&gt;"",CONCATENATE(" ",X2),"")))</f>
+        <f>IF(B2="","",CONCATENATE(Q2," """,R2,IF(K2&lt;&gt;"","{size=+10}",""),TRIM(B2),IF(K2&lt;&gt;"","{/size}",""),S2,"""",IF(X2&lt;&gt;"",CONCATENATE(" ",X2),"")))</f>
         <v/>
       </c>
       <c r="Q2" s="1" t="str">
@@ -2806,7 +2806,7 @@
       </c>
       <c r="N3" s="40"/>
       <c r="P3" t="str">
-        <f t="shared" ref="P3:P66" si="4">IF(B3="","",CONCATENATE(Q3," """,R3,IF(K3&lt;&gt;"","{size=+10}",""),B3,IF(K3&lt;&gt;"","{/size}",""),S3,"""",IF(X3&lt;&gt;"",CONCATENATE(" ",X3),"")))</f>
+        <f t="shared" ref="P3:P66" si="4">IF(B3="","",CONCATENATE(Q3," """,R3,IF(K3&lt;&gt;"","{size=+10}",""),TRIM(B3),IF(K3&lt;&gt;"","{/size}",""),S3,"""",IF(X3&lt;&gt;"",CONCATENATE(" ",X3),"")))</f>
         <v/>
       </c>
       <c r="Q3" s="1" t="str">
@@ -6344,7 +6344,7 @@
         <v/>
       </c>
       <c r="P67" t="str">
-        <f t="shared" ref="P67:P130" si="19">IF(B67="","",CONCATENATE(Q67," """,R67,IF(K67&lt;&gt;"","{size=+10}",""),B67,IF(K67&lt;&gt;"","{/size}",""),S67,"""",IF(X67&lt;&gt;"",CONCATENATE(" ",X67),"")))</f>
+        <f t="shared" ref="P67:P130" si="19">IF(B67="","",CONCATENATE(Q67," """,R67,IF(K67&lt;&gt;"","{size=+10}",""),TRIM(B67),IF(K67&lt;&gt;"","{/size}",""),S67,"""",IF(X67&lt;&gt;"",CONCATENATE(" ",X67),"")))</f>
         <v/>
       </c>
       <c r="Q67" s="1" t="str">
@@ -9810,7 +9810,7 @@
         <v/>
       </c>
       <c r="P131" t="str">
-        <f t="shared" ref="P131:P194" si="32">IF(B131="","",CONCATENATE(Q131," """,R131,IF(K131&lt;&gt;"","{size=+10}",""),B131,IF(K131&lt;&gt;"","{/size}",""),S131,"""",IF(X131&lt;&gt;"",CONCATENATE(" ",X131),"")))</f>
+        <f t="shared" ref="P131:P194" si="32">IF(B131="","",CONCATENATE(Q131," """,R131,IF(K131&lt;&gt;"","{size=+10}",""),TRIM(B131),IF(K131&lt;&gt;"","{/size}",""),S131,"""",IF(X131&lt;&gt;"",CONCATENATE(" ",X131),"")))</f>
         <v/>
       </c>
       <c r="Q131" s="1" t="str">
@@ -13276,7 +13276,7 @@
         <v/>
       </c>
       <c r="P195" t="str">
-        <f t="shared" ref="P195:P251" si="45">IF(B195="","",CONCATENATE(Q195," """,R195,IF(K195&lt;&gt;"","{size=+10}",""),B195,IF(K195&lt;&gt;"","{/size}",""),S195,"""",IF(X195&lt;&gt;"",CONCATENATE(" ",X195),"")))</f>
+        <f t="shared" ref="P195:P251" si="45">IF(B195="","",CONCATENATE(Q195," """,R195,IF(K195&lt;&gt;"","{size=+10}",""),TRIM(B195),IF(K195&lt;&gt;"","{/size}",""),S195,"""",IF(X195&lt;&gt;"",CONCATENATE(" ",X195),"")))</f>
         <v/>
       </c>
       <c r="Q195" s="1" t="str">

</xml_diff>